<commit_message>
Updating dataset type list
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -326,6 +326,12 @@
     <t>dataset_type</t>
   </si>
   <si>
+    <t>HiFi-Slide</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
+  </si>
+  <si>
     <t>SNARE-seq2</t>
   </si>
   <si>
@@ -446,12 +452,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
-    <t>HiFi-Slides</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -1115,7 +1115,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-22T10:40:19-08:00</t>
+    <t>2023-11-24T09:48:56-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>

</xml_diff>

<commit_message>
Updating GeoMx value set
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="274">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -647,6 +647,12 @@
     <t>https://identifiers.org/RRID:SCR_017365</t>
   </si>
   <si>
+    <t>Evident Scientific (Olympus)</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024782</t>
+  </si>
+  <si>
     <t>Keyence</t>
   </si>
   <si>
@@ -770,6 +776,12 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>VS200 Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024783</t>
+  </si>
+  <si>
     <t>Axio Observer 5</t>
   </si>
   <si>
@@ -1061,18 +1073,18 @@
     <t>roi_segmentation_strategy</t>
   </si>
   <si>
-    <t>Automated</t>
+    <t>Manual segmentation</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000305</t>
+  </si>
+  <si>
+    <t>Automated segmentation</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000304</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000305</t>
-  </si>
-  <si>
     <t>anatomical_structure_label</t>
   </si>
   <si>
@@ -1115,7 +1127,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-24T09:48:56-08:00</t>
+    <t>2024-01-05T14:05:37-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1300,103 +1312,103 @@
         <v>96</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
@@ -1404,7 +1416,7 @@
         <v>60</v>
       </c>
       <c r="AN2" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -1419,10 +1431,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$14</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$38</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$39</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1510,10 +1522,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1531,10 +1543,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1552,10 +1564,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1573,42 +1585,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -1672,18 +1684,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -1730,16 +1742,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2">
@@ -1747,13 +1759,13 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2164,7 +2176,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2282,6 +2294,14 @@
         <v>124</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2289,7 +2309,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2297,306 +2317,314 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B30" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B36" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>201</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2614,42 +2642,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2667,26 +2695,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2704,18 +2732,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename "shared_files" to "non_global_files"
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -291,13 +291,16 @@
     </comment>
     <comment ref="AM1" authorId="1">
       <text>
-        <t>(Required) A semicolon separated list of shared files to be included in the
-dataset. The full file path should be used (e.g.,
-"./shared/raw/3146_LabWorksheet.txt; ./shared/raw/3146_GNP_config.ini"). After
-ingest, these files will be copied to the respective locations within the
-dataset directory tree. For example, "./shared/raw/3146_LabWorksheet.txt" will
-be copied to "./raw/3146_LabWorksheet.txt". This field is used for internal
-HuBMAP processing.</t>
+        <t>(Required) A semicolon separated list of non-shared files to be included in the
+dataset. The path assumes the files are located in the "TOP/non-global/"
+directory. For example, for the file is
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
+field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
+these files will be copied to the appropriate locations within the respective
+dataset directory tree. This field is used for internal HuBMAP processing.
+Examples for GeoMx and PhenoCycler are provided in the File Locations
+documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
       </text>
     </comment>
     <comment ref="AN1" authorId="1">
@@ -1106,7 +1109,7 @@
     <t>hybcode_pack_lot_number</t>
   </si>
   <si>
-    <t>shared_files</t>
+    <t>non_global_files</t>
   </si>
   <si>
     <t>metadata_schema_id</t>
@@ -1127,7 +1130,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-05T14:05:37-08:00</t>
+    <t>2024-01-09T13:35:01-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1285,7 +1288,7 @@
     <col min="36" max="36" style="37" width="11.30078125" customWidth="true" bestFit="true"/>
     <col min="37" max="37" style="38" width="19.91796875" customWidth="true" bestFit="true"/>
     <col min="38" max="38" style="39" width="24.71484375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" style="40" width="11.66015625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" style="40" width="15.46484375" customWidth="true" bestFit="true"/>
     <col min="40" max="40" style="41" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Fix dropdown doesn't show
Closes #25
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="318">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -425,6 +425,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
   </si>
   <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -530,6 +536,12 @@
     <t>analyte_class</t>
   </si>
   <si>
+    <t>DNA + RNA</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000327</t>
+  </si>
+  <si>
     <t>Chromatin</t>
   </si>
   <si>
@@ -608,6 +620,18 @@
     <t>acquisition_instrument_vendor</t>
   </si>
   <si>
+    <t>In-House</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
+  </si>
+  <si>
+    <t>BGI Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024848</t>
+  </si>
+  <si>
     <t>Resolve Biosciences</t>
   </si>
   <si>
@@ -638,6 +662,12 @@
     <t>https://identifiers.org/RRID:SCR_023606</t>
   </si>
   <si>
+    <t>GE Healthcare</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_000004</t>
+  </si>
+  <si>
     <t>Sciex</t>
   </si>
   <si>
@@ -650,6 +680,12 @@
     <t>https://identifiers.org/RRID:SCR_017365</t>
   </si>
   <si>
+    <t>Akoya Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023774</t>
+  </si>
+  <si>
     <t>Evident Scientific (Olympus)</t>
   </si>
   <si>
@@ -686,12 +722,24 @@
     <t>https://identifiers.org/RRID:SCR_023609</t>
   </si>
   <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
     <t>Illumina</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_010233</t>
   </si>
   <si>
+    <t>Motic</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024856</t>
+  </si>
+  <si>
     <t>Ionpath</t>
   </si>
   <si>
@@ -719,6 +767,132 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024448</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>Q Exactive UHMR</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020571</t>
+  </si>
+  <si>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020565</t>
+  </si>
+  <si>
+    <t>Zyla 4.2 sCMOS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023610</t>
+  </si>
+  <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
+    <t>QTRAP 5500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020517</t>
+  </si>
+  <si>
+    <t>BZ-X800</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023617</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_014983</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>Hyperion Imaging System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023195</t>
+  </si>
+  <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016381</t>
+  </si>
+  <si>
+    <t>Digital Spatial Profiler</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021660</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
@@ -731,28 +905,28 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
-    <t>NovaSeq X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024569</t>
-  </si>
-  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
-    <t>NanoZoomer 2.0-HT</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021658</t>
-  </si>
-  <si>
-    <t>Lightsheet 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024448</t>
+    <t>PhenoImager Fusion</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023274</t>
+  </si>
+  <si>
+    <t>DM6 B</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024857</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 2.0</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023773</t>
   </si>
   <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
@@ -767,18 +941,18 @@
     <t>https://identifiers.org/RRID:SCR_024449</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
-  </si>
-  <si>
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>TissueScope LE Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024995</t>
+  </si>
+  <si>
     <t>VS200 Slide Scanner</t>
   </si>
   <si>
@@ -809,12 +983,6 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
-    <t>Q Exactive UHMR</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020571</t>
-  </si>
-  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -827,34 +995,16 @@
     <t>https://identifiers.org/RRID:SCR_016387</t>
   </si>
   <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020565</t>
-  </si>
-  <si>
-    <t>Zyla 4.2 sCMOS</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023610</t>
-  </si>
-  <si>
     <t>HiSeq 4000</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
-    <t>QTRAP 5500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020517</t>
-  </si>
-  <si>
-    <t>BZ-X800</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023617</t>
+    <t>Aperio AT2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021256</t>
   </si>
   <si>
     <t>MIBIscope</t>
@@ -863,18 +1013,6 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
-    <t>NextSeq 500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_014983</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -887,36 +1025,6 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
-    <t>Hyperion Imaging System</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023195</t>
-  </si>
-  <si>
-    <t>NovaSeq X Plus</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024568</t>
-  </si>
-  <si>
-    <t>NanoZoomer-SQ</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023763</t>
-  </si>
-  <si>
-    <t>NextSeq 550</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016381</t>
-  </si>
-  <si>
-    <t>Digital Spatial Profiler</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021660</t>
-  </si>
-  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1034,16 +1142,34 @@
     <t>oligo_probe_panel</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 16 BC; PN 1000476</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000308</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Mouse Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-MsWTA-4</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
+  </si>
+  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000306</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 16 BC; PN 1000476</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000308</t>
+    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit - Small; PN 1000365</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
     <t>Custom</t>
@@ -1052,6 +1178,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
   </si>
   <si>
+    <t>NanoString Technologies; GeoMx Human Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-HuWTA-4</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
+  </si>
+  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
   </si>
   <si>
@@ -1130,7 +1262,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-09T13:35:01-08:00</t>
+    <t>2024-03-28T07:39:45-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1250,46 +1382,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="16.6875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="3" width="6.33984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="4" width="23.45703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="5" width="12.28515625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="12.66796875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="10.8984375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="8" width="28.46484375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="9" width="27.87109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="10" width="28.5625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="11" width="27.40234375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="12" width="47.64453125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="13" width="46.48828125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="14" width="16.90625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" style="15" width="9.81640625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" style="16" width="18.53125" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" style="17" width="17.37109375" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="7.8125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="19.44140625" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="36.68359375" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" style="21" width="35.25" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" style="22" width="34.08984375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" style="23" width="24.6328125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" style="24" width="32.2265625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" style="25" width="31.0703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" style="26" width="29.35546875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" style="27" width="28.1953125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" style="28" width="17.39453125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" style="29" width="22.1796875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" style="30" width="8.61328125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" style="31" width="29.17578125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" style="32" width="24.62109375" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" style="33" width="24.86328125" customWidth="true" bestFit="true"/>
-    <col min="33" max="33" style="34" width="22.30078125" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" style="35" width="19.6171875" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" style="36" width="17.0546875" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" style="37" width="11.30078125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" style="38" width="19.91796875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" style="39" width="24.71484375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" style="40" width="15.46484375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" style="41" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="14.39453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="5.46875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="4" width="20.234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="5" width="10.59765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="10.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="7" width="9.40234375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="8" width="24.5546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="9" width="24.0390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="10" width="24.63671875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="11" width="23.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="12" width="41.1015625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="13" width="40.1015625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="14" width="14.5859375" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" style="15" width="8.46484375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" style="16" width="15.984375" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" style="17" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="6.7421875" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" style="19" width="16.76953125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="31.64453125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="30.40625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" style="22" width="29.40625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" style="23" width="21.25" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" style="24" width="27.80078125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" style="25" width="26.80078125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" style="26" width="25.3203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" style="27" width="24.3203125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" style="28" width="15.00390625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" style="29" width="19.1328125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" style="30" width="7.4296875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" style="31" width="25.16796875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" style="32" width="21.23828125" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" style="33" width="21.44921875" customWidth="true" bestFit="true"/>
+    <col min="33" max="33" style="34" width="19.23828125" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" style="35" width="16.921875" customWidth="true" bestFit="true"/>
+    <col min="35" max="35" style="36" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" style="37" width="9.74609375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" style="38" width="17.18359375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" style="39" width="21.3203125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" style="40" width="13.33984375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" style="41" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1306,138 +1438,138 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>207</v>
+        <v>243</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>249</v>
+        <v>293</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>250</v>
+        <v>294</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>251</v>
+        <v>295</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>252</v>
+        <v>296</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>257</v>
+        <v>301</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>258</v>
+        <v>302</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>259</v>
+        <v>303</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>260</v>
+        <v>304</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>261</v>
+        <v>305</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>262</v>
+        <v>306</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>263</v>
+        <v>307</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>265</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>266</v>
+      <c r="D2" t="s" s="5">
+        <v>62</v>
+      </c>
+      <c r="AN2" t="s" s="41">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="25">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$33</formula1>
+      <formula1>'dataset_type'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$11</formula1>
+      <formula1>'analyte_class'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$15</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$39</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1451,7 +1583,7 @@
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
+      <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -1473,7 +1605,7 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'target_retrieval_incubation_time_unit'!$A$1:$A$1</formula1>
+      <formula1>'target_retrieval_incubation_tim'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="V2:V1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -1484,17 +1616,17 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'proteinasek_incubation_time_unit'!$A$1:$A$1</formula1>
+      <formula1>'proteinasek_incubation_time_uni'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="Y2:Y1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'probe_hybridization_time_unit'!$A$1:$A$1</formula1>
+      <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$5</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AB2:AB1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1524,11 +1656,11 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" t="s">
-        <v>217</v>
+      <c r="A1" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1545,11 +1677,11 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" t="s">
-        <v>217</v>
+      <c r="A1" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1559,18 +1691,26 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" t="s">
-        <v>217</v>
+      <c r="A1" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1580,50 +1720,82 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B1" t="s">
-        <v>240</v>
+      <c r="A1" t="s" s="0">
+        <v>275</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>276</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B2" t="s">
-        <v>242</v>
+      <c r="A2" t="s" s="0">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>278</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B3" t="s">
-        <v>244</v>
+      <c r="A3" t="s" s="0">
+        <v>279</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>280</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>245</v>
-      </c>
-      <c r="B4" t="s">
-        <v>246</v>
+      <c r="A4" t="s" s="0">
+        <v>281</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>282</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B5" t="s">
-        <v>248</v>
+      <c r="A5" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -1640,13 +1812,13 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>94</v>
+      <c r="A1" t="s" s="0">
+        <v>98</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>95</v>
+      <c r="A2" t="s" s="0">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1663,13 +1835,13 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>94</v>
+      <c r="A1" t="s" s="0">
+        <v>98</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>95</v>
+      <c r="A2" t="s" s="0">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1686,19 +1858,19 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B1" t="s">
-        <v>254</v>
+      <c r="A1" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>298</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B2" t="s">
-        <v>256</v>
+      <c r="A2" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1715,13 +1887,13 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>94</v>
+      <c r="A1" t="s" s="0">
+        <v>98</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>95</v>
+      <c r="A2" t="s" s="0">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1737,38 +1909,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="17.2578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="79.42578125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.88671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="68.515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D1" t="s">
-        <v>272</v>
+      <c r="A1" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>312</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>314</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>316</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D2" t="s">
-        <v>273</v>
+      <c r="A2" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>315</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -1778,274 +1950,282 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>51</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>55</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>57</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>59</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>61</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>63</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>65</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>67</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>69</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2055,98 +2235,106 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
+      <c r="A1" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>74</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
+      <c r="A2" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>76</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
+      <c r="A3" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>78</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>78</v>
+      <c r="A4" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
+      <c r="A5" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>82</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" t="s">
-        <v>82</v>
+      <c r="A6" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>84</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
+      <c r="A7" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>86</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
+      <c r="A8" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>88</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" t="s">
-        <v>88</v>
+      <c r="A9" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>90</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
+      <c r="A10" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>92</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
+      <c r="A11" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2163,13 +2351,13 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>94</v>
+      <c r="A1" t="s" s="0">
+        <v>98</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>95</v>
+      <c r="A2" t="s" s="0">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2179,130 +2367,178 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+      <c r="A1" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>102</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
+      <c r="A2" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>104</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
+      <c r="A3" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>106</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" t="s">
-        <v>104</v>
+      <c r="A4" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>108</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" t="s">
-        <v>106</v>
+      <c r="A5" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>110</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" t="s">
-        <v>108</v>
+      <c r="A6" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>112</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" t="s">
-        <v>110</v>
+      <c r="A7" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>114</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" t="s">
-        <v>112</v>
+      <c r="A8" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>116</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" t="s">
-        <v>114</v>
+      <c r="A9" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>118</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" t="s">
-        <v>116</v>
+      <c r="A10" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>120</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" t="s">
-        <v>118</v>
+      <c r="A11" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>122</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" t="s">
-        <v>120</v>
+      <c r="A12" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>124</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" t="s">
-        <v>122</v>
+      <c r="A13" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>126</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" t="s">
-        <v>124</v>
+      <c r="A14" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>128</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" t="s">
-        <v>126</v>
+      <c r="A15" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2312,322 +2548,402 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" t="s">
-        <v>129</v>
+      <c r="A1" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>145</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>131</v>
+      <c r="A2" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>147</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" t="s">
-        <v>133</v>
+      <c r="A3" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>149</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" t="s">
-        <v>135</v>
+      <c r="A4" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>151</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B5" t="s">
-        <v>137</v>
+      <c r="A5" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>153</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" t="s">
-        <v>139</v>
+      <c r="A6" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>155</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>141</v>
+      <c r="A7" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>157</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" t="s">
-        <v>143</v>
+      <c r="A8" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>159</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" t="s">
-        <v>145</v>
+      <c r="A9" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>161</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" t="s">
-        <v>147</v>
+      <c r="A10" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>163</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" t="s">
-        <v>149</v>
+      <c r="A11" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>165</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B12" t="s">
-        <v>151</v>
+      <c r="A12" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>167</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B13" t="s">
-        <v>153</v>
+      <c r="A13" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>169</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B14" t="s">
-        <v>155</v>
+      <c r="A14" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>171</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B15" t="s">
-        <v>157</v>
+      <c r="A15" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>173</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B16" t="s">
-        <v>159</v>
+      <c r="A16" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>175</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" t="s">
-        <v>161</v>
+      <c r="A17" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>177</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B18" t="s">
-        <v>163</v>
+      <c r="A18" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>179</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" t="s">
-        <v>165</v>
+      <c r="A19" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>181</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>166</v>
-      </c>
-      <c r="B20" t="s">
-        <v>167</v>
+      <c r="A20" t="s" s="0">
+        <v>182</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>183</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" t="s">
-        <v>169</v>
+      <c r="A21" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>185</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B22" t="s">
-        <v>171</v>
+      <c r="A22" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>187</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>172</v>
-      </c>
-      <c r="B23" t="s">
-        <v>173</v>
+      <c r="A23" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>189</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>174</v>
-      </c>
-      <c r="B24" t="s">
-        <v>175</v>
+      <c r="A24" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>191</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B25" t="s">
-        <v>177</v>
+      <c r="A25" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>193</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>178</v>
-      </c>
-      <c r="B26" t="s">
-        <v>179</v>
+      <c r="A26" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>195</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>180</v>
-      </c>
-      <c r="B27" t="s">
-        <v>181</v>
+      <c r="A27" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>197</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>182</v>
-      </c>
-      <c r="B28" t="s">
-        <v>183</v>
+      <c r="A28" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>199</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" t="s">
-        <v>185</v>
+      <c r="A29" t="s" s="0">
+        <v>200</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>201</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>186</v>
-      </c>
-      <c r="B30" t="s">
-        <v>187</v>
+      <c r="A30" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>203</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>188</v>
-      </c>
-      <c r="B31" t="s">
-        <v>189</v>
+      <c r="A31" t="s" s="0">
+        <v>204</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>205</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B32" t="s">
-        <v>191</v>
+      <c r="A32" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>207</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B33" t="s">
-        <v>193</v>
+      <c r="A33" t="s" s="0">
+        <v>208</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>209</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34" t="s">
-        <v>195</v>
+      <c r="A34" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>211</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B35" t="s">
-        <v>197</v>
+      <c r="A35" t="s" s="0">
+        <v>212</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>213</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>198</v>
-      </c>
-      <c r="B36" t="s">
-        <v>199</v>
+      <c r="A36" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>215</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>200</v>
-      </c>
-      <c r="B37" t="s">
-        <v>201</v>
+      <c r="A37" t="s" s="0">
+        <v>216</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>217</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>202</v>
-      </c>
-      <c r="B38" t="s">
-        <v>203</v>
+      <c r="A38" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>219</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B39" t="s">
-        <v>205</v>
+      <c r="A39" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2644,43 +2960,43 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" t="s">
-        <v>209</v>
+      <c r="A1" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>245</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>211</v>
+      <c r="A2" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>247</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3" t="s">
-        <v>213</v>
+      <c r="A3" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>249</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B4" t="s">
-        <v>215</v>
+      <c r="A4" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>251</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B5" t="s">
-        <v>217</v>
+      <c r="A5" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2697,27 +3013,27 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1" t="s">
-        <v>211</v>
+      <c r="A1" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>247</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B2" t="s">
-        <v>213</v>
+      <c r="A2" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>249</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B3" t="s">
-        <v>215</v>
+      <c r="A3" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2734,19 +3050,19 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B1" t="s">
-        <v>225</v>
+      <c r="A1" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>261</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B2" t="s">
-        <v>227</v>
+      <c r="A2" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor typo fix in "is_custom_probes_used" description
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -226,7 +226,7 @@
       <text>
         <t>(Required) State ("Yes" or "No") whether custom RNA or antibody probes were
 used. If custom probes were used, they must be listed in the
-"custom-probe_set.csv" file.</t>
+"custom_probe_set.csv" file.</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="1">
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="326">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1172,6 +1172,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
   </si>
   <si>
@@ -1280,7 +1286,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-04-01T14:53:07-07:00</t>
+    <t>2024-04-17T14:19:21-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1525,43 +1531,43 @@
         <v>280</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2">
@@ -1569,7 +1575,7 @@
         <v>62</v>
       </c>
       <c r="AN2" t="s" s="41">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -1644,7 +1650,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$9</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AB2:AB1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1738,7 +1744,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1814,6 +1820,14 @@
       </c>
       <c r="B9" t="s" s="0">
         <v>298</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1877,18 +1891,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -1935,16 +1949,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
@@ -1952,13 +1966,13 @@
         <v>62</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the description "mapped_area_value" and "roi_label" columns
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -144,11 +144,13 @@
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) For Visium, this is the area of spots that was covered by tissue
-within the captured area, not the total possible captured area which is fixed.
-For GeoMx this would be the area of the AOI being captured. For HiFi this is the
-summed area of the ROIs in a single flowcell lane. For CosMx, Xenium and
-Resolve, this is the area of the FOV (aka ROI) region being captured.</t>
+        <t>For Visium, this is the area of spots that was covered by tissue within the
+captured area, not the total possible captured area which is fixed. For GeoMx
+this would be the area of the AOI being captured. For HiFi this is the summed
+area of the ROIs in a single flowcell lane. For CosMx and Resolve, this is the
+area of the FOV (aka ROI) region being captured. For Xenium this is the total
+area of the FOV regions (aka ROI) being captured. For Stereo-Seq this is the
+number of beads.</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
@@ -231,9 +233,10 @@
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>(Required) A label for the region of interest (ROI). For Xenium, Resolve and
-CosMx, this is the field of view (FOV) label. For GeoMx this can be found in the
-"Initial Dataset" spreadsheet (download from within Data Analysis Suite).</t>
+        <t>A label for the region of interest. For Resolve and CosMx, this is the field of
+view (FOV) label. For Xenium this is the ID of the region containing the
+analysis. For GeoMx this can be found in the "Initial Dataset" spreadsheet
+(download from within Data Analysis Suite).</t>
       </text>
     </comment>
     <comment ref="AD1" authorId="1">
@@ -315,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="340">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1244,6 +1247,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
   </si>
   <si>
@@ -1322,7 +1331,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-08-03T11:47:19-07:00</t>
+    <t>2024-10-17T13:02:08-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1567,43 +1576,43 @@
         <v>292</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
@@ -1611,7 +1620,7 @@
         <v>66</v>
       </c>
       <c r="AN2" t="s" s="41">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -1686,7 +1695,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$10</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$11</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AB2:AB1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1780,7 +1789,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1864,6 +1873,14 @@
       </c>
       <c r="B10" t="s" s="0">
         <v>312</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -1927,18 +1944,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -1985,16 +2002,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2">
@@ -2002,13 +2019,13 @@
         <v>66</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set "Non-global files" field to optional
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -294,9 +294,9 @@
     </comment>
     <comment ref="AM1" authorId="1">
       <text>
-        <t>(Required) A semicolon separated list of non-shared files to be included in the
-dataset. The path assumes the files are located in the "TOP/non-global/"
-directory. For example, for the file is
+        <t>A semicolon separated list of non-shared files to be included in the dataset.
+The path assumes the files are located in the "TOP/non-global/" directory. For
+example, for the file is
 TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
 field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
 these files will be copied to the appropriate locations within the respective
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="358">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -707,6 +707,12 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Vizgen</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026274</t>
+  </si>
+  <si>
     <t>Standard BioTools (Fluidigm)</t>
   </si>
   <si>
@@ -1064,6 +1070,12 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>MERSCOPE</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000404</t>
+  </si>
+  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -1106,6 +1118,12 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
+    <t>MERSCOPE Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026273</t>
+  </si>
+  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1367,7 +1385,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-01-08T12:47:40-08:00</t>
+    <t>2025-01-22T09:56:35-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1552,103 +1570,103 @@
         <v>116</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2">
@@ -1656,7 +1674,7 @@
         <v>70</v>
       </c>
       <c r="AN2" t="s" s="41">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -1671,10 +1689,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$23</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$24</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$54</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1762,10 +1780,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1783,10 +1801,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1804,18 +1822,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1833,106 +1851,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -1996,18 +2014,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2054,16 +2072,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
@@ -2071,13 +2089,13 @@
         <v>70</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -2568,7 +2586,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2758,6 +2776,14 @@
         <v>162</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2765,7 +2791,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2773,418 +2799,434 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3202,42 +3244,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3255,26 +3297,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3292,18 +3334,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Spatial Transcriptomics metadata template to use updated field descriptions
</commit_message>
<xml_diff>
--- a/geomx-ncounter/latest/geomx-ncounter.xlsx
+++ b/geomx-ncounter/latest/geomx-ncounter.xlsx
@@ -37,279 +37,302 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material stored, prior to this sample being
-processed? For assays applied to tissue sections, this would be how long the
-tissue section (e.g., slide) was stored, prior to the assay beginning (e.g.,
-imaging). For assays applied to suspensions such as sequencing, this would be
-how long the suspension was stored before library construction began.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>For Visium, this is the area of spots that was covered by tissue within the
-captured area, not the total possible captured area which is fixed. For GeoMx
-this would be the area of the AOI being captured. For HiFi this is the summed
-area of the ROIs in a single flowcell lane. For CosMx and Resolve, this is the
-area of the FOV (aka ROI) region being captured. For Xenium this is the total
-area of the FOV regions (aka ROI) being captured. For Stereo-Seq this is the
-number of beads.</t>
+        <t>(Required) The mapped area value, which refers to the specific area covered or
+captured in various assays. For Visium, it is the area of spots covered by
+tissue within the captured area, excluding the total possible captured area. For
+GeoMx, it refers to the area of the AOI being captured. In HiFi, it is the
+summed area of the ROIs in a single flowcell lane. For CosMx and Resolve, it
+indicates the area of the FOV (also known as ROI) region being captured. For
+Xenium, it is the total area of the FOV regions (also known as ROI) being
+captured. For Stereo-Seq, this value represents the number of beads. Example:
+42.25</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) The unit of measurement for the mapping area. For Visium and GeoMx
-this is typically um^2.</t>
+        <t>(Required) The unit of measurement for the mapped area value. If mapping area is
+not specified, this field may be left blank. Example: um^2</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) A unique ID denoting the slide used. This allows users the ability to
+        <t>(Required) The unique identifier assigned to each slide, enabling users to
 determine which tissue sections were processed together on the same slide. It is
-recommended that data providers prefix the ID with the center name, to prevent
-values overlapping across centers.</t>
+recommended that data providers prefix the ID with the center name to prevent
+overlapping values across different centers. Example: VAN0071-PA-1-1_AF</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) The number of distinct fluorescent channels in the image.</t>
+        <t>(Required) The number of distinct fluorescent channels present in the image.
+Example: 3</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>(Required) Will normally be 100 degrees Celsius for RNA assays, and 80 degrees
-Celsius for protein assays.</t>
+        <t>(Required) The incubation temperature required for target retrieval, which is
+typically 100 degrees Celsius for RNA assays and 80 degrees Celsius for protein
+assays. Example: 100</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
         <t>(Required) The duration for which a sample is exposed to a target retrieval
-solution.</t>
+solution. Example: 15</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>(Required) The units for target retrieval incubation time value.</t>
+        <t>(Required) The unit of measurement for the target retrieval incubation time
+value. If no incubation time is specified, this field may be left blank.
+Example: minute</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>The amount or concentration of the enzyme Proteinase K within a sample (in
-ug/ml).</t>
+        <t>The concentration of the enzyme Proteinase K within a sample, measured in
+micrograms per milliliter (ug/ml). Example: 10</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>The duration for which a sample is exposed to Proteinase K.</t>
+        <t>The duration for which a sample is incubated with Proteinase K. Example: 15</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
       <text>
-        <t>The units for proteinaseK incubation time value.</t>
+        <t>The unit of measurement for the proteinaseK incubation time value. If no
+incubation time is specified, this field may be left blank. Example: minute</t>
       </text>
     </comment>
     <comment ref="Y1" authorId="1">
       <text>
-        <t>(Required) How many hours were the oligo-conjugated RNA or oligo-conjugated
-antibody probes hybridized with the sample?</t>
+        <t>(Required) The duration for which the oligo-conjugated RNA or oligo-conjugated
+antibody probes were hybridized with the sample. Example: 30</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>(Required) The units for probe hybridization time value.</t>
+        <t>(Required) The unit of measurement for the probe hybridization time value. If
+the hybridization time is not specified, this field may be left blank. Example:
+minute</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
-        <t>(Required) This is the probe panel used to target genes and/or proteins. In
-cases where there is a core panel and add-on modules, the core panel should be
-selected here. If additional panels are used, then they must be included in the
-"additional_panels_used.csv" file that's uploaded with the dataset.</t>
+        <t>(Required) The oligo probe panel used to target genes and/or proteins. If there
+is a core panel along with add-on modules, the core panel should be selected in
+this field. Any additional panels utilized should be documented in the
+"additional_panels_used.csv" file, which must be uploaded alongside the dataset.
+Example: 10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="1">
       <text>
-        <t>(Required) State ("Yes" or "No") whether custom RNA or antibody probes were
-used. If custom probes were used, they must be listed in the
-"custom_probe_set.csv" file.</t>
+        <t>(Required) Indicates whether custom RNA or antibody probes were utilized in the
+assay. If custom probes were employed, they should be documented in the
+"custom_probe_set.csv" file. Example: No</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>A label for the region of interest. For Resolve and CosMx, this is the field of
-view (FOV) label. For Xenium this is the ID of the region containing the
-analysis. For GeoMx this can be found in the "Initial Dataset" spreadsheet
-(download from within Data Analysis Suite).</t>
+        <t>(Required) The label for the region of interest (ROI). For Resolve and CosMx,
+this corresponds to the field of view (FOV) label. In the case of Xenium, it
+refers to the ID of the region containing the analysis. For GeoMx, this
+information can be located in the "Initial Dataset" spreadsheet, which can be
+downloaded from within the Data Analysis Suite. Example: Decidua</t>
       </text>
     </comment>
     <comment ref="AD1" authorId="1">
       <text>
-        <t>(Required) Was the image segmented. For GeoMx this refers to whether
-segmentation was used to split ROIs (regions of interest) into AOIs (areas of
-interest).</t>
+        <t>(Required) Indicates whether ROI (Region of Interest) segmentation was performed
+on the image. For GeoMx, this refers to the use of segmentation to divide ROIs
+into AOIs (Areas of Interest). Answer with "Yes" or "No" value. Example: Yes</t>
       </text>
     </comment>
     <comment ref="AE1" authorId="1">
       <text>
-        <t>The method of segmentation that was applied in a GeoMx assay. If an overlay was
-used the overlay image needs to be included in the dataset upload.</t>
+        <t>The segmentation strategy employed in a GeoMx assay. If an overlay was utilized,
+ensure that the overlay image is included in the dataset upload. Example:
+Automated segmentation</t>
       </text>
     </comment>
     <comment ref="AF1" authorId="1">
       <text>
-        <t>The overarching anatomical structure.</t>
+        <t>The label for the overarching anatomical structure. If the anatomical structure
+is not applicable or not specified, this field may be left blank. Example:
+Kidney</t>
       </text>
     </comment>
     <comment ref="AG1" authorId="1">
       <text>
-        <t>The ontology ID for the parent structure. Typically this would be an UBERON ID.</t>
+        <t>The ontology ID associated with the anatomical structure, typically represented
+by an UBERON ID. Example: UBERON:0002113</t>
       </text>
     </comment>
     <comment ref="AH1" authorId="1">
       <text>
-        <t>(Required) State what cell type(s) or functional tissue unit was targeted in
-this ROI/AOI.</t>
+        <t>(Required) The label for the targeted entity, indicating the specific cell
+type(s) or functional tissue unit that was targeted within this Region of
+Interest (ROI) or Area of Interest (AOI). Example: ROI-001</t>
       </text>
     </comment>
     <comment ref="AI1" authorId="1">
       <text>
-        <t>The ontology ID for the targeted entity.</t>
+        <t>The ontology ID associated with the targeted entity. If no specific entity is
+targeted, this field may be left blank. Example: CL:0000540</t>
       </text>
     </comment>
     <comment ref="AJ1" authorId="1">
       <text>
-        <t>(Required) This is the ID for the area of interest (AOI) in a GeoMx dataset.
-From "Initial Dataset" spreadsheet (download from within Data Analysis Suite),
-e.g. 9a828e39-43d8-4051-9bcc-581a520a85d4.</t>
+        <t>(Required) The unique identifier for the area of interest (AOI) within a GeoMx
+dataset. This ID can be found in the "Initial Dataset" spreadsheet, which can be
+downloaded from the Data Analysis Suite. Example:
+9a828e39-43d8-4051-9bcc-581a520a85d4</t>
       </text>
     </comment>
     <comment ref="AK1" authorId="1">
       <text>
-        <t>(Required) Is the sequencing reaction run in replicate, "Yes" or "No". If "Yes",
-FASTQ files in dataset need to be merged.</t>
+        <t>(Required) Indicates whether the sequencing reaction was run in replicate. If
+"Yes," the corresponding FASTQ files in the dataset should be merged for
+analysis. Example: Yes</t>
       </text>
     </comment>
     <comment ref="AL1" authorId="1">
       <text>
-        <t>(Required) Enter the lot number noted within the LabWorksheet.txt file (and used
-in downstream nCounter processing).</t>
+        <t>(Required) The lot number found within the LabWorksheet.txt file, which is used
+in subsequent nCounter processing.</t>
       </text>
     </comment>
     <comment ref="AM1" authorId="1">
       <text>
-        <t>A semicolon separated list of non-shared files to be included in the dataset.
-The path assumes the files are located in the "TOP/non-global/" directory. For
-example, for the file is
-TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
-field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
-these files will be copied to the appropriate locations within the respective
-dataset directory tree. This field is used for internal HuBMAP processing.
-Examples for GeoMx and PhenoCycler are provided in the File Locations
-documentation:
-https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
+        <t>Specifies a semicolon-separated list of non-global files that are to be included
+in the dataset. The file paths assume that the files are located in the
+"TOP/non-global/" directory. For instance, if the file is located at
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson, the value for
+this field would be "./lab_processed/images/1-tissue-boundary.geojson". Once
+ingested, these files will be copied to their appropriate locations within the
+respective dataset directory tree. This field is intended for internal HuBMAP
+processing. Examples for GeoMx and PhenoCycler are provided in the File
+Locations documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee
+Example: ./lab_processed/images/1-tissue-boundary.geojson</t>
       </text>
     </comment>
     <comment ref="AN1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -318,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="467">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -344,34 +367,172 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -380,36 +541,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000434</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -440,16 +571,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -458,30 +583,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -512,18 +619,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -536,12 +631,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -554,34 +643,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -725,6 +796,12 @@
     <t>https://identifiers.org/RRID:SCR_027007</t>
   </si>
   <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -839,12 +916,24 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -878,6 +967,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -986,6 +1081,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1064,6 +1165,12 @@
     <t>https://identifiers.org/RRID:SCR_016381</t>
   </si>
   <si>
+    <t>Axio Zoom.V16</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027090</t>
+  </si>
+  <si>
     <t>Digital Spatial Profiler</t>
   </si>
   <si>
@@ -1100,6 +1207,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1190,6 +1303,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1214,6 +1330,18 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>solariX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027095</t>
+  </si>
+  <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1226,6 +1354,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1250,6 +1384,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1361,40 +1501,124 @@
     <t>oligo_probe_panel</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Next GEM Single Cell Fixed RNA Mouse Transcriptome Probe Kit, 64 rxns; PN 1000492</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Prime 5K Human Pan Tissue &amp; Pathways Panel; PN 1000724</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000426</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Mouse Multi-Tissue Atlassing Panel; PN 1000627</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000442</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit v2.0 - Small; PN 1000667</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000431</t>
+  </si>
+  <si>
+    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Human 6K Discovery Panel (RNA, 6175 Plex); PN 121500041</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000455</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Mouse Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-M-USCP-1KP-R</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000457</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Custom Gene Expression Panel (51-100 genes); PN 1000561</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000444</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Human Colon Gene Expression Panel; PN 1000642</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000446</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000436</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit - Small; PN 1000365</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Hs WTX RNA Panel Kit, 2 slides: PN 121500047</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000453</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Human Lung Gene Expression Panel; PN 1000601</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000443</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (Protein, 64 Plex); PN CMX-M-Neuro-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000437</t>
+  </si>
+  <si>
     <t>NanoString Technologies; GeoMx Mouse Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-MsWTA-4</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Next GEM Single Cell Fixed RNA Mouse Transcriptome Probe Kit, 64 rxns; PN 1000492</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
-  </si>
-  <si>
-    <t>10x Genomics; Xenium Prime 5K Human Pan Tissue &amp; Pathways Panel; PN 1000724</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000426</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit v2.0 - Small; PN 1000667</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000431</t>
+    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (RNA, 1000 Plex); PN CMX-M-NEUP-R</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000452</t>
   </si>
   <si>
     <t>Custom</t>
@@ -1409,34 +1633,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
-  </si>
-  <si>
     <t>10x Genomics; Xenium Human Multi-Tissue and Cancer Panel v1; PN 1000626</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000395</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
-  </si>
-  <si>
-    <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000436</t>
+    <t>10x Genomics; Xenium Custom Gene Expression Panel (up to 50 genes); PN 1000464</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000445</t>
   </si>
   <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
@@ -1445,30 +1651,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000306</t>
   </si>
   <si>
-    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit - Small; PN 1000365</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
-  </si>
-  <si>
     <t>NanoString Technologies; CosMx Human Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-H-USCP-1KP-R</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000430</t>
   </si>
   <si>
-    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (Protein, 64 Plex); PN CMX-M-Neuro-64P-P</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000437</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000382</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Hs Univ Cell (RNA, 1000 Plex); PN 121500002</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000454</t>
+  </si>
+  <si>
     <t>is_custom_probes_used</t>
   </si>
   <si>
@@ -1535,7 +1735,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-04T14:01:33-07:00</t>
+    <t>2025-10-22T11:06:00-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1711,126 +1911,126 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>314</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>315</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>327</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>328</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>330</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>331</v>
+        <v>370</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>336</v>
+        <v>375</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>337</v>
+        <v>376</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>338</v>
+        <v>377</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>339</v>
+        <v>378</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>340</v>
+        <v>379</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>341</v>
+        <v>380</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>342</v>
+        <v>381</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>343</v>
+        <v>382</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>344</v>
+        <v>383</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>345</v>
+        <v>384</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>383</v>
+        <v>442</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>384</v>
+        <v>443</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>385</v>
+        <v>444</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>386</v>
+        <v>445</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>391</v>
+        <v>450</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>392</v>
+        <v>451</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>393</v>
+        <v>452</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>394</v>
+        <v>453</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>395</v>
+        <v>454</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>396</v>
+        <v>455</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>397</v>
+        <v>456</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>398</v>
+        <v>457</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>399</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="AN2" t="s" s="41">
-        <v>400</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="25">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$42</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1839,10 +2039,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$27</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1899,7 +2099,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$18</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$28</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AB2:AB1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1930,10 +2130,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -1951,10 +2151,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -1972,18 +2172,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>325</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -1993,7 +2193,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2001,146 +2201,226 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>347</v>
+        <v>386</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>348</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>350</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>351</v>
+        <v>390</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>352</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>353</v>
+        <v>392</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>354</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>355</v>
+        <v>394</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>356</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>357</v>
+        <v>396</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>358</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>359</v>
+        <v>398</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>360</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>361</v>
+        <v>400</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>362</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>363</v>
+        <v>402</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>364</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>365</v>
+        <v>404</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>366</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>367</v>
+        <v>406</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>368</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>369</v>
+        <v>408</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>370</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>371</v>
+        <v>410</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>372</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>373</v>
+        <v>412</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>374</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>375</v>
+        <v>414</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>376</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>377</v>
+        <v>416</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>378</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>379</v>
+        <v>418</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>380</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>381</v>
+        <v>420</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>382</v>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>422</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>424</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>426</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>428</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>430</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>434</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>436</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>438</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>440</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -2158,12 +2438,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2181,12 +2461,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2204,18 +2484,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>387</v>
+        <v>446</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>388</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>389</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>390</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -2233,12 +2513,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2262,30 +2542,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>401</v>
+        <v>460</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>402</v>
+        <v>461</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>404</v>
+        <v>463</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>406</v>
+        <v>465</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>403</v>
+        <v>462</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>405</v>
+        <v>464</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>407</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -2295,7 +2575,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2635,6 +2915,70 @@
       </c>
       <c r="B42" t="s" s="0">
         <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2652,130 +2996,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2793,12 +3137,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2808,7 +3152,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2816,218 +3160,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>138</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>144</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>176</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>178</v>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3037,7 +3405,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3045,546 +3413,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>181</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>185</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>187</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>189</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>191</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>195</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>197</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>199</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>201</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>203</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>207</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>209</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>211</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>213</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>215</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>217</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>219</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>221</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>223</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>225</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>227</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>229</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>231</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>235</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>237</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>239</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>241</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>243</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>247</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>249</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>251</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>253</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>255</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>257</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>259</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>261</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>262</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>263</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>265</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>267</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>269</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>271</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>273</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>275</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>276</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>279</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>280</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>281</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>283</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>284</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>285</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>287</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>288</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>289</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>290</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>291</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>292</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>293</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>294</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>295</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>153</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>154</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>296</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>297</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>299</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>301</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>303</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>304</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>305</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>306</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>307</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>309</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>311</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>313</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>337</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>339</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3602,42 +4042,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>318</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>319</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>320</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>321</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>323</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>325</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3655,26 +4095,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>318</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>319</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>320</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>321</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>323</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3692,18 +4132,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>332</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>333</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>334</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>335</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>